<commit_message>
Add coding to autowrite values
</commit_message>
<xml_diff>
--- a/00_data.xlsx
+++ b/00_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://asnonline-my.sharepoint.com/personal/kpivert_asn-online_org/Documents/Documents/01_gh/ay-2023_match_draft/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{E365A7CA-A04B-4D71-ABEE-78172769C6E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CC92F02-0487-4843-8221-B21EEA2BED57}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{E365A7CA-A04B-4D71-ABEE-78172769C6E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B77A9E35-4C8D-41F3-94D1-B5A10CE4E263}"/>
   <bookViews>
     <workbookView xWindow="34935" yWindow="1500" windowWidth="21600" windowHeight="11385" xr2:uid="{334DF07A-342B-4ED7-9A0E-540FCDF41B3B}"/>
   </bookViews>
@@ -204,6 +204,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -505,9 +509,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CD96B11-8B47-4052-B5A5-24FCAF52EB7D}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P22" sqref="P22"/>
+      <selection pane="topRight" activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -613,7 +617,7 @@
         <v>484</v>
       </c>
       <c r="P2" s="1">
-        <v>484</v>
+        <v>500</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
@@ -663,7 +667,7 @@
         <v>335</v>
       </c>
       <c r="P3" s="1">
-        <v>335</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -713,7 +717,7 @@
         <v>149</v>
       </c>
       <c r="P4" s="1">
-        <v>149</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -763,7 +767,7 @@
         <v>0.69199999999999995</v>
       </c>
       <c r="P5" s="2">
-        <v>0.69199999999999995</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -813,7 +817,7 @@
         <v>178</v>
       </c>
       <c r="P6" s="1">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -863,7 +867,7 @@
         <v>93</v>
       </c>
       <c r="P7" s="1">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -913,7 +917,7 @@
         <v>85</v>
       </c>
       <c r="P8" s="1">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -963,7 +967,7 @@
         <v>0.52200000000000002</v>
       </c>
       <c r="P9" s="2">
-        <v>0.52200000000000002</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
@@ -1063,7 +1067,7 @@
         <v>337</v>
       </c>
       <c r="P11" s="1">
-        <v>337</v>
+        <v>320</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -1113,7 +1117,7 @@
         <v>315</v>
       </c>
       <c r="P12" s="1">
-        <v>315</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
@@ -1163,7 +1167,7 @@
         <v>1</v>
       </c>
       <c r="P13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
@@ -1213,7 +1217,7 @@
         <v>21</v>
       </c>
       <c r="P14" s="1">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
@@ -1263,7 +1267,7 @@
         <v>335</v>
       </c>
       <c r="P15" s="1">
-        <v>335</v>
+        <v>300</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
@@ -1313,7 +1317,7 @@
         <v>96</v>
       </c>
       <c r="P16" s="1">
-        <v>96</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
@@ -1363,7 +1367,7 @@
         <v>56</v>
       </c>
       <c r="P17" s="1">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
@@ -1413,7 +1417,7 @@
         <v>63</v>
       </c>
       <c r="P18" s="1">
-        <v>63</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
@@ -1463,7 +1467,7 @@
         <v>120</v>
       </c>
       <c r="P19" s="1">
-        <v>120</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>